<commit_message>
shift left 2 implemented and functional
</commit_message>
<xml_diff>
--- a/Proj1_control_signals.xlsx
+++ b/Proj1_control_signals.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="78">
   <si>
     <t xml:space="preserve">Instruction</t>
   </si>
@@ -92,6 +92,12 @@
     <t xml:space="preserve">RegDst</t>
   </si>
   <si>
+    <t xml:space="preserve">Branch</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ALUOp</t>
+  </si>
+  <si>
     <t xml:space="preserve">Note: these are example control signals from the text and your skeleton code; you will need to add more control signals; you may rename any control signals, except those given in the skeleton code.</t>
   </si>
   <si>
@@ -248,85 +254,157 @@
     <t xml:space="preserve">addiu</t>
   </si>
   <si>
+    <t xml:space="preserve">"001001"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">addu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"000000"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"100001"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0 [addi does NOT read from memory]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0 [addi does NOT write to memory]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 [addi writes back to a register]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0 [does not branch</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10 [read as an R-instr]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">add</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"100000"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0010 [the alu will perform an add of A and B]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0 [does not branch]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">and</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"100100"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">andi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"001100"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lui</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"001111"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lw</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"100011"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"100111"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">xor</t>
+  </si>
+  <si>
     <t xml:space="preserve">“000000”</t>
   </si>
   <si>
-    <t xml:space="preserve">“100001”</t>
-  </si>
-  <si>
-    <t xml:space="preserve">add</t>
-  </si>
-  <si>
-    <t xml:space="preserve">“100000”</t>
-  </si>
-  <si>
-    <t xml:space="preserve">subi</t>
+    <t xml:space="preserve">“100110”</t>
+  </si>
+  <si>
+    <t xml:space="preserve">xori</t>
+  </si>
+  <si>
+    <t xml:space="preserve">“001110”</t>
+  </si>
+  <si>
+    <t xml:space="preserve">“------”</t>
+  </si>
+  <si>
+    <t xml:space="preserve">or</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"100101"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ori</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"001101"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">slt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"101010"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">slti</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"001010"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sll</t>
+  </si>
+  <si>
+    <t xml:space="preserve">srl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"000010"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sra</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"000011"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sw</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"101011"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sub</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"100010"</t>
   </si>
   <si>
     <t xml:space="preserve">subu</t>
   </si>
   <si>
-    <t xml:space="preserve">sub</t>
-  </si>
-  <si>
-    <t xml:space="preserve">and</t>
-  </si>
-  <si>
-    <t xml:space="preserve">“100100”</t>
-  </si>
-  <si>
-    <t xml:space="preserve">andi</t>
-  </si>
-  <si>
-    <t xml:space="preserve">“001100”</t>
-  </si>
-  <si>
-    <t xml:space="preserve">“------”</t>
-  </si>
-  <si>
-    <t xml:space="preserve">nor</t>
-  </si>
-  <si>
-    <t xml:space="preserve">xori</t>
-  </si>
-  <si>
-    <t xml:space="preserve">xor</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ori</t>
-  </si>
-  <si>
-    <t xml:space="preserve">or</t>
-  </si>
-  <si>
-    <t xml:space="preserve">lui</t>
-  </si>
-  <si>
-    <t xml:space="preserve">lw</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sw</t>
-  </si>
-  <si>
     <t xml:space="preserve">beq</t>
   </si>
   <si>
+    <t xml:space="preserve">"000100"</t>
+  </si>
+  <si>
     <t xml:space="preserve">bne</t>
   </si>
   <si>
-    <t xml:space="preserve">slt</t>
-  </si>
-  <si>
-    <t xml:space="preserve">slti</t>
-  </si>
-  <si>
-    <t xml:space="preserve">srl</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sll</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sra</t>
+    <t xml:space="preserve">"000101"</t>
   </si>
   <si>
     <t xml:space="preserve">j</t>
@@ -452,36 +530,115 @@
 </styleSheet>
 </file>
 
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <xdr:twoCellAnchor editAs="absolute">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>655920</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>154800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1980000</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>165960</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="0" name="Image 1" descr=""/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId1"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1414080" y="6250680"/>
+          <a:ext cx="7268040" cy="1535040"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="absolute">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>841680</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>154080</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>2254320</xdr:colOff>
+      <xdr:row>68</xdr:row>
+      <xdr:rowOff>91800</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="1" name="Image 2" descr=""/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId2"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1599840" y="7964280"/>
+          <a:ext cx="7356600" cy="5081400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:O28"/>
+  <dimension ref="A1:Q28"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="3" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="D1" activeCellId="0" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="C10" activeCellId="0" sqref="C10"/>
+      <selection pane="bottomRight" activeCell="E10" activeCellId="0" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.8203125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.7890625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="9.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="14.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="12.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="49.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="39.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="9.8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="14.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="12.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="49.8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="39.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="32.51"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="30.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="30.8"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="27"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="45.5"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="10" style="1" width="10.83"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="10" style="1" width="10.8"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -505,8 +662,10 @@
       <c r="M1" s="3"/>
       <c r="N1" s="3"/>
       <c r="O1" s="3"/>
-    </row>
-    <row r="2" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="P1" s="3"/>
+      <c r="Q1" s="3"/>
+    </row>
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2"/>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -528,189 +687,600 @@
       <c r="I2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="J2" s="4" t="s">
+      <c r="J2" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="K2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="L2" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="J3" s="4" t="s">
-        <v>20</v>
+        <v>21</v>
+      </c>
+      <c r="L3" s="4" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>25</v>
+        <v>27</v>
+      </c>
+      <c r="D5" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="I5" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>26</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D6" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="I6" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="K6" s="1" t="n">
+        <v>10</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>27</v>
+        <v>37</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D7" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="I7" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>28</v>
+        <v>39</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>29</v>
+        <v>41</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>22</v>
+        <v>42</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>30</v>
+        <v>15</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>31</v>
+        <v>43</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>32</v>
+        <v>44</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>33</v>
+        <v>15</v>
+      </c>
+      <c r="D10" s="1" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>34</v>
+        <v>45</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D11" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="I11" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="K11" s="1" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>35</v>
+        <v>47</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D12" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="I12" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="J12" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="K12" s="1" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>36</v>
+        <v>50</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>37</v>
+        <v>53</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D14" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="I14" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="J14" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="K14" s="1" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>38</v>
+        <v>55</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>39</v>
+        <v>57</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D16" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="I16" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="J16" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="K16" s="1" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>40</v>
+        <v>59</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>41</v>
+        <v>61</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D18" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="I18" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="J18" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="K18" s="1" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>42</v>
+        <v>62</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="D19" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="I19" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="J19" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="K19" s="1" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
-        <v>43</v>
+        <v>64</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D20" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="I20" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="J20" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="K20" s="1" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>44</v>
+        <v>66</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>45</v>
+        <v>68</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="D22" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="I22" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="J22" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="K22" s="1" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
-        <v>46</v>
+        <v>70</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D23" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="I23" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="J23" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="K23" s="1" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
-        <v>47</v>
+        <v>71</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
-        <v>48</v>
+        <v>73</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
-        <v>49</v>
+        <v>75</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
-        <v>50</v>
+        <v>76</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="s">
-        <v>51</v>
+        <v>77</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D28" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="H28" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="I28" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="J28" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="K28" s="1" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -718,7 +1288,7 @@
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:O1"/>
+    <mergeCell ref="D1:Q1"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -727,5 +1297,6 @@
     <oddHeader/>
     <oddFooter/>
   </headerFooter>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>